<commit_message>
Added 2x10 shrouded header connector
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14320" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Part</t>
   </si>
@@ -199,16 +199,31 @@
   </si>
   <si>
     <t>ABS07L-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>Shrouded Header</t>
+  </si>
+  <si>
+    <t>CNN HEADDER 2.54mm 10POS GOLD</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>SBH11-PBPC-D05-ST-BK</t>
+  </si>
+  <si>
+    <t>S9169-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,6 +1049,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1061,7 +1077,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="278">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1632,79 +1647,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="1"/>
+    <col min="11" max="13" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.1" customHeight="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:14" ht="14" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1">
+      <c r="A2" s="14"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -1788,7 +1803,7 @@
         <v>9.5214700000000008</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30">
+    <row r="5" spans="1:14">
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30">
+    <row r="9" spans="1:14" ht="28">
       <c r="B9" s="6" t="s">
         <v>56</v>
       </c>
@@ -1960,8 +1975,8 @@
         <v>0.66149999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30">
-      <c r="B10" s="17" t="s">
+    <row r="10" spans="1:14">
+      <c r="B10" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1996,12 +2011,34 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="I11"/>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="J11"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="K11" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.29849999999999999</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0.21590000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="I12"/>
@@ -2029,7 +2066,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="14.1" customHeight="1">
+    <row r="16" spans="1:14" ht="14" customHeight="1">
       <c r="I16"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>

</xml_diff>

<commit_message>
Added Schottky diode to mBom
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14320" windowHeight="16660"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22460" windowHeight="18140"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>Part</t>
   </si>
@@ -214,6 +214,30 @@
   </si>
   <si>
     <t>S9169-ND</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>0603/SOD-523F</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 500MA 0603</t>
+  </si>
+  <si>
+    <t>Comchip Technology</t>
+  </si>
+  <si>
+    <t>CDBU0530</t>
+  </si>
+  <si>
+    <t>641-1285-1-ND</t>
+  </si>
+  <si>
+    <t>20V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1650,16 +1674,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2040,15 +2064,43 @@
         <v>0.21590000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="I12"/>
+    <row r="12" spans="1:14" ht="14" customHeight="1">
+      <c r="B12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
       <c r="J12"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="K12" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.216</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0.11</v>
+      </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="14" customHeight="1">
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -2061,6 +2113,9 @@
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14">
+      <c r="F15" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>

</xml_diff>

<commit_message>
Updated Marionette_connections, ABM7 library, component selection spreadsheet, and bill of materials
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="111">
   <si>
     <t>Part</t>
   </si>
@@ -170,7 +170,7 @@
     <t>CP-047A-ND</t>
   </si>
   <si>
-    <t>16th MHz Crystal</t>
+    <t>ABM7</t>
   </si>
   <si>
     <t>2-SMD</t>
@@ -327,16 +327,38 @@
   </si>
   <si>
     <t>490-6477-1-ND</t>
+  </si>
+  <si>
+    <t>8.06k Resistor</t>
+  </si>
+  <si>
+    <t>8.06k</t>
+  </si>
+  <si>
+    <t>0.1W</t>
+  </si>
+  <si>
+    <t>RES SMD 8.06K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Panasonic electronic Components</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF8061V</t>
+  </si>
+  <si>
+    <t>P8.06KHCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -454,7 +476,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,6 +547,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -544,10 +570,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -562,8 +588,8 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.6599190283401"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.8380566801619"/>
     <col collapsed="false" hidden="true" max="10" min="10" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="6.49797570850202"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="5.49797570850202"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="7.48987854251012"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.62753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="8.83400809716599"/>
   </cols>
   <sheetData>
@@ -1150,17 +1176,55 @@
       <c r="I17" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="K17" s="1" t="n">
+      <c r="K17" s="18" t="n">
         <v>0.32</v>
       </c>
-      <c r="L17" s="1" t="n">
+      <c r="L17" s="18" t="n">
         <v>0.28</v>
       </c>
-      <c r="M17" s="1" t="n">
+      <c r="M17" s="18" t="n">
         <v>0.14</v>
       </c>
-      <c r="N17" s="1" t="n">
+      <c r="N17" s="18" t="n">
         <v>0.092</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="18" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="N18" s="18" t="n">
+        <v>0.00416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SWD connector to mBom
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="22220" windowWidth="26260" windowHeight="15280" tabRatio="480"/>
+    <workbookView xWindow="7220" yWindow="18180" windowWidth="25600" windowHeight="16060" tabRatio="480"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="124">
   <si>
     <t>Part</t>
   </si>
@@ -357,9 +357,6 @@
     <t>ABS25-32.768KHZ-6-T</t>
   </si>
   <si>
-    <t>35-10240-1-ND</t>
-  </si>
-  <si>
     <t>11uF Capacitor</t>
   </si>
   <si>
@@ -379,6 +376,21 @@
   </si>
   <si>
     <t>490-6072-1-ND</t>
+  </si>
+  <si>
+    <t>535-10240-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BOX HEADER, 0.050 10 POS</t>
+  </si>
+  <si>
+    <t>CNC Tech</t>
+  </si>
+  <si>
+    <t>3220-10-0100-00</t>
+  </si>
+  <si>
+    <t>1175-1627-ND</t>
   </si>
 </sst>
 </file>
@@ -490,21 +502,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -528,6 +525,21 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,708 +872,737 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="11"/>
-    <col min="4" max="5" width="8.83203125" style="6"/>
-    <col min="6" max="6" width="34.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" style="6" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="6"/>
+    <col min="4" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="7">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="2">
         <v>100</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="7">
         <v>0.92</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="7">
         <v>0.81699999999999995</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="7">
         <v>0.64500000000000002</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="7">
         <v>0.39679999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="7">
         <v>15.75</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="7">
         <v>14.318</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="7">
         <v>12.170299999999999</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="7">
         <v>9.5214700000000008</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="7">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="7">
         <v>0.47299999999999998</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="7">
         <v>0.378</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="7">
         <v>0.3024</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="7">
         <v>1.26</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="7">
         <v>1.2250000000000001</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="7">
         <v>1.49</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="7">
         <v>1.24</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="7">
         <v>0.94</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="7">
         <v>0.97</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="7">
         <v>0.752</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="7">
         <v>0.57379999999999998</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="7">
         <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="4">
         <v>0.96</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="4">
         <v>0.84699999999999998</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="4">
         <v>0.7</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="4">
         <v>0.66149999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0.31900000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0.64</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0.29849999999999999</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0.21590000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="14" customHeight="1">
+      <c r="B12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0.216</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14" customHeight="1">
+      <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="N13" s="7">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L14" s="7">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="N14" s="7">
+        <v>1.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0.115</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0.31630000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="14" customHeight="1">
+      <c r="B16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="M16" s="7">
+        <v>6.93E-2</v>
+      </c>
+      <c r="N16" s="7">
+        <v>4.2079999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N17" s="8">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="8">
+        <v>1.14E-2</v>
+      </c>
+      <c r="N18" s="8">
+        <v>4.1599999999999996E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="L10" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="M10" s="12">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="N10" s="12">
-        <v>0.31900000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="B11" s="6" t="s">
+      <c r="C19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M19" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="N19" s="1">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0.64</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="M11" s="12">
-        <v>0.29849999999999999</v>
-      </c>
-      <c r="N11" s="12">
-        <v>0.21590000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="14" customHeight="1">
-      <c r="B12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0.31</v>
-      </c>
-      <c r="M12" s="12">
-        <v>0.216</v>
-      </c>
-      <c r="N12" s="12">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="14" customHeight="1">
-      <c r="B13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="L13" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="M13" s="12">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="N13" s="12">
-        <v>6.3E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="B14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="L14" s="12">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="M14" s="12">
-        <v>1.8700000000000001E-2</v>
-      </c>
-      <c r="N14" s="12">
-        <v>1.0200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="B15" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="K15" s="12">
-        <v>0.17</v>
-      </c>
-      <c r="L15" s="12">
-        <v>0.115</v>
-      </c>
-      <c r="M15" s="12">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="N15" s="12">
-        <v>0.31630000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="14" customHeight="1">
-      <c r="B16" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="L16" s="12">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="M16" s="12">
-        <v>6.93E-2</v>
-      </c>
-      <c r="N16" s="12">
-        <v>4.2079999999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="K17" s="13">
-        <v>0.32</v>
-      </c>
-      <c r="L17" s="13">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="M17" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="N17" s="13">
-        <v>9.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="B18" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="K18" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="13">
-        <v>1.14E-2</v>
-      </c>
-      <c r="N18" s="13">
-        <v>4.1599999999999996E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="K19" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="L19" s="6">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M19" s="6">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="N19" s="6">
-        <v>3.6999999999999998E-2</v>
+      <c r="F20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
This time I really added the pushbutton datasheet and bom info
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="18180" windowWidth="25600" windowHeight="16060" tabRatio="480"/>
+    <workbookView xWindow="4180" yWindow="1480" windowWidth="30760" windowHeight="17000" tabRatio="480"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>Part</t>
   </si>
@@ -192,21 +192,6 @@
     <t>535-9840-1-ND</t>
   </si>
   <si>
-    <t>Shrouded Header</t>
-  </si>
-  <si>
-    <t>CNN HEADDER 2.54mm 10POS GOLD</t>
-  </si>
-  <si>
-    <t>Sullins Connector Solutions</t>
-  </si>
-  <si>
-    <t>SBH11-PBPC-D05-ST-BK</t>
-  </si>
-  <si>
-    <t>S9169-ND</t>
-  </si>
-  <si>
     <t>Schottky Diode</t>
   </si>
   <si>
@@ -391,6 +376,27 @@
   </si>
   <si>
     <t>1175-1627-ND</t>
+  </si>
+  <si>
+    <t>SWD Header</t>
+  </si>
+  <si>
+    <t>Push Button</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>C&amp;K Components</t>
+  </si>
+  <si>
+    <t>PTS645SM43SMTR92 LFS</t>
+  </si>
+  <si>
+    <t>CKN9112CT-ND</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -526,19 +532,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -874,15 +880,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="6"/>
+    <col min="3" max="3" width="13.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.83203125" style="1"/>
     <col min="6" max="6" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -893,19 +899,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -914,33 +920,33 @@
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -1198,25 +1204,25 @@
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K10" s="7">
         <v>0.6</v>
@@ -1231,316 +1237,316 @@
         <v>0.31900000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="14" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="K11" s="7">
-        <v>0.64</v>
+        <v>0.4</v>
       </c>
       <c r="L11" s="7">
-        <v>0.44500000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="M11" s="7">
-        <v>0.29849999999999999</v>
+        <v>0.216</v>
       </c>
       <c r="N11" s="7">
-        <v>0.21590000000000001</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="14" customHeight="1">
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="N12" s="7">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="L12" s="7">
-        <v>0.31</v>
-      </c>
-      <c r="M12" s="7">
-        <v>0.216</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="14" customHeight="1">
-      <c r="B13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>73</v>
+      <c r="F13" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K13" s="7">
         <v>0.1</v>
       </c>
       <c r="L13" s="7">
-        <v>2.5000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M13" s="7">
-        <v>1.1599999999999999E-2</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="N13" s="7">
-        <v>6.3E-3</v>
+        <v>1.0200000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K14" s="7">
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="L14" s="7">
-        <v>4.1000000000000002E-2</v>
+        <v>0.115</v>
       </c>
       <c r="M14" s="7">
-        <v>1.8700000000000001E-2</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="N14" s="7">
-        <v>1.0200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>0.31630000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="14" customHeight="1">
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="M15" s="7">
+        <v>6.93E-2</v>
+      </c>
+      <c r="N15" s="7">
+        <v>4.2079999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="K15" s="7">
-        <v>0.17</v>
-      </c>
-      <c r="L15" s="7">
-        <v>0.115</v>
-      </c>
-      <c r="M15" s="7">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0.31630000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="14" customHeight="1">
-      <c r="B16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="L16" s="7">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="M16" s="7">
-        <v>6.93E-2</v>
-      </c>
-      <c r="N16" s="7">
-        <v>4.2079999999999999E-2</v>
+        <v>95</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N16" s="8">
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K17" s="8">
-        <v>0.32</v>
-      </c>
-      <c r="L17" s="8">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="M17" s="8">
-        <v>0.14000000000000001</v>
+        <v>1.14E-2</v>
       </c>
       <c r="N17" s="8">
-        <v>9.1999999999999998E-2</v>
+        <v>4.1599999999999996E-3</v>
       </c>
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="K18" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="8">
-        <v>1.14E-2</v>
-      </c>
-      <c r="N18" s="8">
-        <v>4.1599999999999996E-3</v>
+        <v>93</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M18" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="N18" s="1">
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>117</v>
@@ -1549,60 +1555,60 @@
         <v>118</v>
       </c>
       <c r="K19" s="1">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="L19" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="M19" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>0.35</v>
       </c>
       <c r="N19" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K20" s="1">
-        <v>0.48</v>
+        <v>0.21</v>
       </c>
       <c r="L20" s="1">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="M20" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="N20" s="1">
-        <v>0.25</v>
+        <v>0.18</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
Added super cap to mBom and its datasheet
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="1480" windowWidth="30760" windowHeight="17000" tabRatio="480"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="16500" windowHeight="15580" tabRatio="480"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="133">
   <si>
     <t>Part</t>
   </si>
@@ -397,6 +397,27 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Super Cap</t>
+  </si>
+  <si>
+    <t>220mF</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>CAP 220MF -20% +80% 3.3V SMD</t>
+  </si>
+  <si>
+    <t>Elna America</t>
+  </si>
+  <si>
+    <t>DCK-3R3E224U-E</t>
+  </si>
+  <si>
+    <t>604-1007-ND</t>
   </si>
 </sst>
 </file>
@@ -407,7 +428,7 @@
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -427,6 +448,22 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -503,8 +540,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -532,23 +571,25 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -878,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -899,19 +940,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -920,33 +961,33 @@
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="9"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="12"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -1596,21 +1637,57 @@
         <v>125</v>
       </c>
     </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0.52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding current limiting resistors for RGB LED
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="480" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="1320" yWindow="23820" windowWidth="25660" windowHeight="14620" tabRatio="480"/>
   </bookViews>
   <sheets>
-    <sheet name="mBom" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="mBom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="160">
   <si>
     <t>Part</t>
   </si>
@@ -191,7 +195,7 @@
     <t>ABS25</t>
   </si>
   <si>
-    <t>4-SOJ </t>
+    <t>4-SOJ</t>
   </si>
   <si>
     <t>CRYSTAL 32.768KHZ 6PF SMD</t>
@@ -365,7 +369,7 @@
     <t>SWD Header</t>
   </si>
   <si>
-    <t> BOX HEADER, 0.050 10 POS</t>
+    <t>BOX HEADER, 0.050 10 POS</t>
   </si>
   <si>
     <t>CNC Tech</t>
@@ -465,41 +469,47 @@
   </si>
   <si>
     <t>490-10148-1-ND</t>
+  </si>
+  <si>
+    <t>5.1 ohm resistor</t>
+  </si>
+  <si>
+    <t>.1W</t>
+  </si>
+  <si>
+    <t>RES SMD 5.1 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW06035R10JNEA</t>
+  </si>
+  <si>
+    <t>541-5.1GCT-ND</t>
+  </si>
+  <si>
+    <t>68 ohm resistor</t>
+  </si>
+  <si>
+    <t>RES SMD 68 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC1608J680CS</t>
+  </si>
+  <si>
+    <t>1276-5034-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -521,373 +531,657 @@
     </fill>
   </fills>
   <borders count="6">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="medium"/>
-      <top style="medium"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="medium"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:N24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.49797570850202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.331983805668"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.336032388664"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8380566801619"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.0040485829959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.502024291498"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="3" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="8.83400809716599"/>
+    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-    </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="9" t="n">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="12">
         <v>1</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="12">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="n">
+      <c r="M2" s="12">
         <v>100</v>
       </c>
-      <c r="N2" s="10" t="n">
+      <c r="N2" s="13">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:14">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0"/>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="3">
         <v>0.92</v>
       </c>
-      <c r="L3" s="3" t="n">
-        <v>0.817</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>0.645</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>0.3968</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L3" s="3">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.39679999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="3">
         <v>15.75</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="3">
         <v>14.318</v>
       </c>
-      <c r="M4" s="3" t="n">
-        <v>12.1703</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>9.52147</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" s="3">
+        <v>12.170299999999999</v>
+      </c>
+      <c r="N4" s="3">
+        <v>9.5214700000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="0"/>
       <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="0"/>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="3" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>0.473</v>
-      </c>
-      <c r="M5" s="3" t="n">
+      <c r="K5" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="M5" s="3">
         <v>0.378</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="3">
         <v>0.3024</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:14">
       <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="0"/>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="3">
         <v>1.26</v>
       </c>
-      <c r="L6" s="3" t="n">
-        <v>1.225</v>
+      <c r="L6" s="3">
+        <v>1.2250000000000001</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>26</v>
@@ -896,158 +1190,153 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:14">
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="0"/>
       <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="4" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="3">
         <v>1.49</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="3">
         <v>1.24</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="3">
         <v>0.94</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:14">
       <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="0"/>
       <c r="E8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="K8" s="3">
         <v>0.97</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="3">
         <v>0.752</v>
       </c>
-      <c r="M8" s="3" t="n">
-        <v>0.5738</v>
-      </c>
-      <c r="N8" s="3" t="n">
-        <v>0.408</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="3">
+        <v>0.57379999999999998</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.40799999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="0"/>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="13" t="n">
+      <c r="K9" s="6">
         <v>0.96</v>
       </c>
-      <c r="L9" s="13" t="n">
-        <v>0.847</v>
-      </c>
-      <c r="M9" s="13" t="n">
+      <c r="L9" s="6">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="M9" s="6">
         <v>0.7</v>
       </c>
-      <c r="N9" s="13" t="n">
-        <v>0.6615</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N9" s="6">
+        <v>0.66149999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="0"/>
       <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="3">
         <v>0.6</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="3">
         <v>0.5</v>
       </c>
-      <c r="M10" s="3" t="n">
-        <v>0.399</v>
-      </c>
-      <c r="N10" s="3" t="n">
-        <v>0.319</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M10" s="3">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.31900000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="0"/>
       <c r="E11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1063,20 +1352,20 @@
       <c r="I11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="K11" s="3">
         <v>0.4</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="3">
         <v>0.31</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="3">
         <v>0.216</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="N11" s="3">
         <v>0.11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:14">
       <c r="B12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1089,32 +1378,32 @@
       <c r="E12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="K12" s="3">
         <v>0.1</v>
       </c>
-      <c r="L12" s="3" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="M12" s="3" t="n">
-        <v>0.0116</v>
-      </c>
-      <c r="N12" s="3" t="n">
-        <v>0.0063</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="B13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1133,26 +1422,26 @@
       <c r="G13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="K13" s="3">
         <v>0.1</v>
       </c>
-      <c r="L13" s="3" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="M13" s="3" t="n">
-        <v>0.0187</v>
-      </c>
-      <c r="N13" s="3" t="n">
-        <v>0.0102</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="B14" s="1" t="s">
         <v>83</v>
       </c>
@@ -1165,32 +1454,32 @@
       <c r="E14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="5" t="s">
         <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="3">
         <v>0.17</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="3">
         <v>0.115</v>
       </c>
-      <c r="M14" s="3" t="n">
-        <v>0.546</v>
-      </c>
-      <c r="N14" s="3" t="n">
-        <v>0.3163</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M14" s="3">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.31630000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15" s="1" t="s">
         <v>89</v>
       </c>
@@ -1203,32 +1492,32 @@
       <c r="E15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="3" t="n">
+      <c r="K15" s="3">
         <v>0.2</v>
       </c>
-      <c r="L15" s="3" t="n">
-        <v>0.136</v>
-      </c>
-      <c r="M15" s="3" t="n">
-        <v>0.0693</v>
-      </c>
-      <c r="N15" s="3" t="n">
-        <v>0.04208</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L15" s="3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="M15" s="3">
+        <v>6.93E-2</v>
+      </c>
+      <c r="N15" s="3">
+        <v>4.2079999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="B16" s="1" t="s">
         <v>95</v>
       </c>
@@ -1241,32 +1530,32 @@
       <c r="E16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K16" s="3" t="n">
+      <c r="K16" s="3">
         <v>0.32</v>
       </c>
-      <c r="L16" s="3" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="M16" s="3" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="N16" s="3" t="n">
-        <v>0.092</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L16" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N16" s="3">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -1279,32 +1568,32 @@
       <c r="E17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="K17" s="3" t="n">
+      <c r="K17" s="3">
         <v>0.1</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M17" s="3" t="n">
-        <v>0.0114</v>
-      </c>
-      <c r="N17" s="3" t="n">
-        <v>0.00416</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M17" s="3">
+        <v>1.14E-2</v>
+      </c>
+      <c r="N17" s="3">
+        <v>4.1599999999999996E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
       <c r="B18" s="1" t="s">
         <v>108</v>
       </c>
@@ -1329,26 +1618,24 @@
       <c r="I18" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K18" s="3" t="n">
+      <c r="K18" s="3">
         <v>0.2</v>
       </c>
-      <c r="L18" s="3" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="M18" s="3" t="n">
-        <v>0.066</v>
-      </c>
-      <c r="N18" s="3" t="n">
-        <v>0.037</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L18" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M18" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="N18" s="3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
+      <c r="C19" s="1"/>
       <c r="F19" s="1" t="s">
         <v>116</v>
       </c>
@@ -1361,26 +1648,24 @@
       <c r="I19" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="K19" s="3" t="n">
+      <c r="K19" s="3">
         <v>0.48</v>
       </c>
-      <c r="L19" s="3" t="n">
+      <c r="L19" s="3">
         <v>0.45</v>
       </c>
-      <c r="M19" s="3" t="n">
+      <c r="M19" s="3">
         <v>0.35</v>
       </c>
-      <c r="N19" s="3" t="n">
+      <c r="N19" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:14">
       <c r="B20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
+      <c r="C20" s="1"/>
       <c r="F20" s="1" t="s">
         <v>121</v>
       </c>
@@ -1393,24 +1678,24 @@
       <c r="I20" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K20" s="3" t="n">
+      <c r="K20" s="3">
         <v>0.21</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="L20" s="3">
         <v>0.2</v>
       </c>
-      <c r="M20" s="3" t="n">
+      <c r="M20" s="3">
         <v>0.18</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:14">
       <c r="B21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="0"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>127</v>
       </c>
@@ -1429,20 +1714,20 @@
       <c r="I21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K21" s="3" t="n">
+      <c r="K21" s="3">
         <v>1.41</v>
       </c>
-      <c r="L21" s="3" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="M21" s="3" t="n">
+      <c r="L21" s="3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="M21" s="3">
         <v>0.83</v>
       </c>
-      <c r="N21" s="3" t="n">
+      <c r="N21" s="3">
         <v>0.52</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:14">
       <c r="B22" s="1" t="s">
         <v>133</v>
       </c>
@@ -1461,52 +1746,52 @@
       <c r="J22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="3" t="n">
+      <c r="K22" s="3">
         <v>1.79</v>
       </c>
-      <c r="L22" s="3" t="n">
-        <v>1.16</v>
-      </c>
-      <c r="M22" s="3" t="n">
+      <c r="L22" s="3">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="M22" s="3">
         <v>1.03</v>
       </c>
-      <c r="N22" s="3" t="n">
-        <v>0.677</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N22" s="3">
+        <v>0.67700000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="5" t="s">
         <v>141</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="3" t="n">
+      <c r="K23" s="3">
         <v>0.95</v>
       </c>
-      <c r="L23" s="3" t="n">
-        <v>0.839</v>
-      </c>
-      <c r="M23" s="3" t="n">
-        <v>0.6934</v>
-      </c>
-      <c r="N23" s="3" t="n">
-        <v>0.54775</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="3">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0.54774999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24" s="1" t="s">
         <v>144</v>
       </c>
@@ -1519,51 +1804,126 @@
       <c r="E24" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="5" t="s">
         <v>147</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="K24" s="3" t="n">
+      <c r="K24" s="3">
         <v>0.1</v>
       </c>
-      <c r="L24" s="3" t="n">
-        <v>0.061</v>
-      </c>
-      <c r="M24" s="3" t="n">
-        <v>0.0281</v>
-      </c>
-      <c r="N24" s="3" t="n">
-        <v>0.0153</v>
+      <c r="L24" s="3">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>2.81E-2</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1.5299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1">
+        <v>68</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:N1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding male right angle headers
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="23820" windowWidth="25660" windowHeight="14620" tabRatio="480"/>
+    <workbookView xWindow="5320" yWindow="3640" windowWidth="25660" windowHeight="14620" tabRatio="480"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="169">
   <si>
     <t>Part</t>
   </si>
@@ -499,6 +499,33 @@
   </si>
   <si>
     <t>1276-5034-1-ND</t>
+  </si>
+  <si>
+    <t>Male header</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A DUAL 4POS GOLD</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>961204-5604-AR</t>
+  </si>
+  <si>
+    <t>3M9478-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER .100" DUAL R/A 10POS</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>PRPC005DBAN-M71RC</t>
+  </si>
+  <si>
+    <t>S2111EC-05-ND</t>
   </si>
 </sst>
 </file>
@@ -617,26 +644,26 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -992,64 +1019,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="12">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="7">
         <v>1</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="7">
         <v>10</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="7">
         <v>100</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="8">
         <v>1000</v>
       </c>
     </row>
@@ -1905,19 +1932,77 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0.39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
Added another angle male header
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="172">
   <si>
     <t>Part</t>
   </si>
@@ -516,16 +516,25 @@
     <t>3M9478-ND</t>
   </si>
   <si>
-    <t>CONN HEADER .100" DUAL R/A 10POS</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>PRPC005DBAN-M71RC</t>
-  </si>
-  <si>
-    <t>S2111EC-05-ND</t>
+    <t>CONN HEADER DUAL 8 POS RA 2.54</t>
+  </si>
+  <si>
+    <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t>732-5353-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER .100" DUAL R/A 20POS</t>
+  </si>
+  <si>
+    <t>PRPC010DBAN-M71RC</t>
+  </si>
+  <si>
+    <t>S2111EC-10-ND</t>
   </si>
 </sst>
 </file>
@@ -650,19 +659,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -996,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1019,19 +1028,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -1040,33 +1049,33 @@
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="7">
         <v>1</v>
       </c>
@@ -1966,43 +1975,72 @@
         <v>160</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H28" s="1" t="s">
         <v>167</v>
+      </c>
+      <c r="H28" s="1">
+        <v>61300821021</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>168</v>
       </c>
       <c r="K28" s="3">
-        <v>0.78</v>
-      </c>
-      <c r="L28" s="3">
         <v>0.7</v>
       </c>
+      <c r="L28" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="M28" s="3">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="N28" s="3">
-        <v>0.39</v>
+        <v>0.63</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1.08</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0.54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
Added 1.8V LDO to bom
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="3640" windowWidth="25660" windowHeight="14620" tabRatio="480"/>
+    <workbookView xWindow="820" yWindow="23080" windowWidth="25660" windowHeight="14620" tabRatio="480"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="178">
   <si>
     <t>Part</t>
   </si>
@@ -535,6 +535,24 @@
   </si>
   <si>
     <t>S2111EC-10-ND</t>
+  </si>
+  <si>
+    <t>AAT3221</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>IC REG LDO 1.8V 0.15A SOT23-5</t>
+  </si>
+  <si>
+    <t>Skyworks Solutions Inc</t>
+  </si>
+  <si>
+    <t>AAT3221IGV-1.8-T1</t>
+  </si>
+  <si>
+    <t>863-1508-1-ND</t>
   </si>
 </sst>
 </file>
@@ -659,19 +677,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1005,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1028,19 +1046,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -1049,33 +1067,33 @@
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="9"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="12"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="7">
         <v>1</v>
       </c>
@@ -2028,19 +2046,51 @@
         <v>0.54</v>
       </c>
     </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="N30" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
Added 16MHz crystal to mBom
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="175">
   <si>
     <t>Part</t>
   </si>
@@ -174,24 +174,9 @@
     <t>CP-047A-ND</t>
   </si>
   <si>
-    <t>ABM7</t>
-  </si>
-  <si>
-    <t>2-SMD</t>
-  </si>
-  <si>
-    <t>CRYSTAL 16MHZ 18PF SMD</t>
-  </si>
-  <si>
     <t>Abracom Corporation</t>
   </si>
   <si>
-    <t>ABM7-16.000MHZ-D2Y-T</t>
-  </si>
-  <si>
-    <t>535-9840-1-ND</t>
-  </si>
-  <si>
     <t>ABS25</t>
   </si>
   <si>
@@ -553,6 +538,12 @@
   </si>
   <si>
     <t>863-1508-1-ND</t>
+  </si>
+  <si>
+    <t>NX3225</t>
+  </si>
+  <si>
+    <t>4-SMD</t>
   </si>
 </sst>
 </file>
@@ -677,19 +668,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1025,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1046,19 +1037,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -1067,33 +1058,33 @@
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="7">
         <v>1</v>
       </c>
@@ -1316,60 +1307,60 @@
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>173</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="K9" s="6">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="L9" s="6">
-        <v>0.84699999999999998</v>
+        <v>0.84</v>
       </c>
       <c r="M9" s="6">
-        <v>0.7</v>
+        <v>0.69</v>
       </c>
       <c r="N9" s="6">
-        <v>0.66149999999999998</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K10" s="3">
         <v>0.6</v>
@@ -1386,25 +1377,25 @@
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="K11" s="3">
         <v>0.4</v>
@@ -1421,28 +1412,28 @@
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="H12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="I12" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="K12" s="3">
         <v>0.1</v>
@@ -1459,28 +1450,28 @@
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="K13" s="3">
         <v>0.1</v>
@@ -1497,28 +1488,28 @@
     </row>
     <row r="14" spans="1:14">
       <c r="B14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="K14" s="3">
         <v>0.17</v>
@@ -1535,28 +1526,28 @@
     </row>
     <row r="15" spans="1:14">
       <c r="B15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="K15" s="3">
         <v>0.2</v>
@@ -1573,28 +1564,28 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="K16" s="3">
         <v>0.32</v>
@@ -1611,28 +1602,28 @@
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="I17" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="K17" s="3">
         <v>0.1</v>
@@ -1649,28 +1640,28 @@
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="K18" s="3">
         <v>0.2</v>
@@ -1687,20 +1678,20 @@
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K19" s="3">
         <v>0.48</v>
@@ -1717,20 +1708,20 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K20" s="3">
         <v>0.21</v>
@@ -1742,31 +1733,31 @@
         <v>0.18</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="2:14">
       <c r="B21" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="K21" s="3">
         <v>1.41</v>
@@ -1783,22 +1774,22 @@
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="K22" s="3">
         <v>1.79</v>
@@ -1815,19 +1806,19 @@
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>33</v>
@@ -1847,28 +1838,28 @@
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="K24" s="3">
         <v>0.1</v>
@@ -1885,28 +1876,28 @@
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K25" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1923,28 +1914,28 @@
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1">
         <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K26" s="3">
         <v>0.1</v>
@@ -1961,19 +1952,19 @@
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K27" s="3">
         <v>0.33</v>
@@ -1990,19 +1981,19 @@
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H28" s="1">
         <v>61300821021</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K28" s="3">
         <v>0.7</v>
@@ -2019,19 +2010,19 @@
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K29" s="3">
         <v>1.08</v>
@@ -2048,22 +2039,22 @@
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="K30" s="3">
         <v>0.17</v>
@@ -2080,17 +2071,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
updated bom and apparently gantt chart
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="208">
   <si>
     <t>Part</t>
   </si>
@@ -573,6 +573,72 @@
   </si>
   <si>
     <t>475-2512-1-ND </t>
+  </si>
+  <si>
+    <t>100 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>meh </t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/8W 0603 </t>
+  </si>
+  <si>
+    <t>Vishay Beyschlag</t>
+  </si>
+  <si>
+    <t>MCT06030C1000FP500</t>
+  </si>
+  <si>
+    <t>MCT0603-100-CFCT-ND</t>
+  </si>
+  <si>
+    <t>649 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>RES SMD 649 OHM 1% 1/10W 0603 </t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Incx</t>
+  </si>
+  <si>
+    <t>RMCF0603FT649R</t>
+  </si>
+  <si>
+    <t>RMCF0603FT649RCT-ND </t>
+  </si>
+  <si>
+    <t>59k Ohm Resistor</t>
+  </si>
+  <si>
+    <t>59k</t>
+  </si>
+  <si>
+    <t>RES SMD 59K OHM 1% 1/10W 0603 </t>
+  </si>
+  <si>
+    <t>ERJ-3EKF5902V</t>
+  </si>
+  <si>
+    <t>P59.0KHCT-ND </t>
+  </si>
+  <si>
+    <t>10pF Capacitor</t>
+  </si>
+  <si>
+    <t>10pf</t>
+  </si>
+  <si>
+    <t>CAP CER 10PF 50V C0G 0402 </t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>C1005C0G1H100C050BA</t>
+  </si>
+  <si>
+    <t>445-4896-1-ND </t>
   </si>
 </sst>
 </file>
@@ -782,10 +848,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N37" activeCellId="0" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1907,7 +1973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="14" t="s">
         <v>180</v>
       </c>
@@ -1944,6 +2010,152 @@
       <c r="N32" s="3" t="n">
         <f aca="false">-C320603</f>
         <v>-0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L33" s="3" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="M33" s="3" t="n">
+        <v>0.0408</v>
+      </c>
+      <c r="N33" s="3" t="n">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>649</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="M34" s="3" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="N34" s="3" t="n">
+        <v>0.00384</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="M35" s="3" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="N35" s="3" t="n">
+        <v>0.00416</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="K36" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="M36" s="3" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="N36" s="3" t="n">
+        <v>0.0063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited 0.05" header info
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="25040" windowWidth="26420" windowHeight="14120" tabRatio="986"/>
+    <workbookView xWindow="1780" yWindow="29060" windowWidth="26420" windowHeight="14120" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -645,13 +645,13 @@
     <t>445-4896-1-ND</t>
   </si>
   <si>
-    <t>CONN HEADER .050" 22PS DL PCB AU</t>
-  </si>
-  <si>
-    <t>GRPB112VWVN-RC</t>
-  </si>
-  <si>
-    <t>S9015E-11-ND</t>
+    <t>CONN HEADER .050" 14PS DL PCB AU</t>
+  </si>
+  <si>
+    <t>GRPB072VWVN-RC</t>
+  </si>
+  <si>
+    <t>S9015E-07-ND</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -754,21 +754,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -790,14 +775,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,63 +1132,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35:Q36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="7.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" style="6"/>
+    <col min="1" max="1" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="14" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
       <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
@@ -2201,26 +2201,26 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="7">
+      <c r="A2" s="14"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="2">
         <v>100</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="3">
         <v>1000</v>
       </c>
       <c r="O2"/>
@@ -3236,39 +3236,39 @@
     </row>
     <row r="3" spans="1:1024">
       <c r="A3"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="13">
+      <c r="J3" s="4"/>
+      <c r="K3" s="8">
         <v>0.92</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="8">
         <v>0.81699999999999995</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="8">
         <v>0.64500000000000002</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="8">
         <v>0.39679999999999999</v>
       </c>
       <c r="O3"/>
@@ -4284,39 +4284,39 @@
     </row>
     <row r="4" spans="1:1024">
       <c r="A4"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="13">
+      <c r="J4" s="4"/>
+      <c r="K4" s="8">
         <v>15.75</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="8">
         <v>14.318</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="8">
         <v>12.170299999999999</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="8">
         <v>9.5214700000000008</v>
       </c>
       <c r="O4"/>
@@ -5332,37 +5332,37 @@
     </row>
     <row r="5" spans="1:1024">
       <c r="A5"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="13">
+      <c r="J5" s="4"/>
+      <c r="K5" s="8">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="8">
         <v>0.47299999999999998</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="8">
         <v>0.378</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="8">
         <v>0.3024</v>
       </c>
       <c r="O5"/>
@@ -6378,39 +6378,39 @@
     </row>
     <row r="6" spans="1:1024">
       <c r="A6"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="13">
+      <c r="J6" s="4"/>
+      <c r="K6" s="8">
         <v>1.26</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="8">
         <v>1.2250000000000001</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O6"/>
@@ -7426,39 +7426,39 @@
     </row>
     <row r="7" spans="1:1024">
       <c r="A7"/>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="13">
+      <c r="J7" s="4"/>
+      <c r="K7" s="8">
         <v>1.49</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="8">
         <v>1.24</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="8">
         <v>0.94</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O7"/>
@@ -8474,39 +8474,39 @@
     </row>
     <row r="8" spans="1:1024">
       <c r="A8"/>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="13">
+      <c r="J8" s="4"/>
+      <c r="K8" s="8">
         <v>0.97</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="8">
         <v>0.752</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="8">
         <v>0.57379999999999998</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="8">
         <v>0.40799999999999997</v>
       </c>
       <c r="O8"/>
@@ -9522,39 +9522,39 @@
     </row>
     <row r="9" spans="1:1024">
       <c r="A9"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="14">
+      <c r="J9" s="4"/>
+      <c r="K9" s="9">
         <v>0.95</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="9">
         <v>0.84</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="9">
         <v>0.69</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="9">
         <v>0.54</v>
       </c>
       <c r="O9"/>
@@ -10570,39 +10570,39 @@
     </row>
     <row r="10" spans="1:1024">
       <c r="A10"/>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="13">
+      <c r="J10" s="4"/>
+      <c r="K10" s="8">
         <v>0.6</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="8">
         <v>0.5</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="8">
         <v>0.39900000000000002</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="8">
         <v>0.31900000000000001</v>
       </c>
       <c r="O10"/>
@@ -11618,39 +11618,39 @@
     </row>
     <row r="11" spans="1:1024">
       <c r="A11"/>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="13">
+      <c r="J11" s="4"/>
+      <c r="K11" s="8">
         <v>0.4</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="8">
         <v>0.31</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="8">
         <v>0.216</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="8">
         <v>0.11</v>
       </c>
       <c r="O11"/>
@@ -12666,41 +12666,41 @@
     </row>
     <row r="12" spans="1:1024">
       <c r="A12"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="13">
+      <c r="J12" s="4"/>
+      <c r="K12" s="8">
         <v>0.1</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="8">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="8">
         <v>6.3E-3</v>
       </c>
       <c r="O12"/>
@@ -13716,41 +13716,41 @@
     </row>
     <row r="13" spans="1:1024">
       <c r="A13"/>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="13">
+      <c r="J13" s="4"/>
+      <c r="K13" s="8">
         <v>0.1</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="8">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="8">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="8">
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="O13"/>
@@ -14766,41 +14766,41 @@
     </row>
     <row r="14" spans="1:1024">
       <c r="A14"/>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="13">
+      <c r="J14" s="4"/>
+      <c r="K14" s="8">
         <v>0.17</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="8">
         <v>0.115</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="8">
         <v>0.54600000000000004</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="8">
         <v>0.31630000000000003</v>
       </c>
       <c r="O14"/>
@@ -15816,41 +15816,41 @@
     </row>
     <row r="15" spans="1:1024">
       <c r="A15"/>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="13">
+      <c r="J15" s="4"/>
+      <c r="K15" s="8">
         <v>0.2</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="8">
         <v>6.93E-2</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="8">
         <v>4.2079999999999999E-2</v>
       </c>
       <c r="O15"/>
@@ -16866,41 +16866,41 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16"/>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="13">
+      <c r="J16" s="4"/>
+      <c r="K16" s="8">
         <v>0.32</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="8">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="O16"/>
@@ -17916,41 +17916,41 @@
     </row>
     <row r="17" spans="1:1024">
       <c r="A17"/>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="13">
+      <c r="J17" s="4"/>
+      <c r="K17" s="8">
         <v>0.1</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="8">
         <v>1.14E-2</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="8">
         <v>4.1599999999999996E-3</v>
       </c>
       <c r="O17"/>
@@ -18966,41 +18966,41 @@
     </row>
     <row r="18" spans="1:1024">
       <c r="A18"/>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="13">
+      <c r="J18" s="4"/>
+      <c r="K18" s="8">
         <v>0.2</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="8">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="8">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="O18"/>
@@ -20015,695 +20015,698 @@
       <c r="AMJ18"/>
     </row>
     <row r="19" spans="1:1024">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="13">
+      <c r="J19" s="4"/>
+      <c r="K19" s="8">
         <v>0.48</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="8">
         <v>0.45</v>
       </c>
-      <c r="M19" s="13">
+      <c r="M19" s="8">
         <v>0.35</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="8">
         <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:1024">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="13">
+      <c r="J20" s="4"/>
+      <c r="K20" s="8">
         <v>0.21</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="8">
         <v>0.2</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="8">
         <v>0.18</v>
       </c>
-      <c r="N20" s="13" t="s">
+      <c r="N20" s="8" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:1024">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="13">
+      <c r="J21" s="4"/>
+      <c r="K21" s="8">
         <v>1.41</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="8">
         <v>1.1100000000000001</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="8">
         <v>0.83</v>
       </c>
-      <c r="N21" s="13">
+      <c r="N21" s="8">
         <v>0.52</v>
       </c>
     </row>
     <row r="22" spans="1:1024">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9" t="s">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="8">
         <v>1.79</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="8">
         <v>1.1599999999999999</v>
       </c>
-      <c r="M22" s="13">
+      <c r="M22" s="8">
         <v>1.03</v>
       </c>
-      <c r="N22" s="13">
+      <c r="N22" s="8">
         <v>0.67700000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:1024" ht="14" customHeight="1">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="12" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="13">
+      <c r="J23" s="4"/>
+      <c r="K23" s="8">
         <v>0.95</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L23" s="8">
         <v>0.83899999999999997</v>
       </c>
-      <c r="M23" s="13">
+      <c r="M23" s="8">
         <v>0.69340000000000002</v>
       </c>
-      <c r="N23" s="13">
+      <c r="N23" s="8">
         <v>0.54774999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:1024">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="13">
+      <c r="J24" s="4"/>
+      <c r="K24" s="8">
         <v>0.1</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="8">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M24" s="13">
+      <c r="M24" s="8">
         <v>2.81E-2</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="8">
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:1024">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="13">
+      <c r="J25" s="4"/>
+      <c r="K25" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="13" t="s">
+      <c r="M25" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="8">
         <v>0.02</v>
       </c>
     </row>
     <row r="26" spans="1:1024">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="4">
         <v>68</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="13">
+      <c r="J26" s="4"/>
+      <c r="K26" s="8">
         <v>0.1</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="8">
         <v>0.01</v>
       </c>
-      <c r="M26" s="13">
+      <c r="M26" s="8">
         <v>0.01</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="8">
         <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:1024">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="13">
+      <c r="J27" s="4"/>
+      <c r="K27" s="8">
         <v>0.33</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="8">
         <v>0.32</v>
       </c>
-      <c r="M27" s="13">
+      <c r="M27" s="8">
         <v>0.22</v>
       </c>
-      <c r="N27" s="13">
+      <c r="N27" s="8">
         <v>0.15</v>
       </c>
     </row>
     <row r="28" spans="1:1024">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="4">
         <v>61300821021</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="13">
+      <c r="J28" s="4"/>
+      <c r="K28" s="8">
         <v>0.7</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="L28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="13">
+      <c r="M28" s="8">
         <v>0.63</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1024">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="13">
+      <c r="J29" s="4"/>
+      <c r="K29" s="8">
         <v>1.08</v>
       </c>
-      <c r="L29" s="13">
+      <c r="L29" s="8">
         <v>0.97</v>
       </c>
-      <c r="M29" s="13">
+      <c r="M29" s="8">
         <v>0.79</v>
       </c>
-      <c r="N29" s="13">
+      <c r="N29" s="8">
         <v>0.54</v>
       </c>
     </row>
     <row r="30" spans="1:1024">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9" t="s">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="13">
+      <c r="J30" s="4"/>
+      <c r="K30" s="8">
         <v>0.17</v>
       </c>
-      <c r="L30" s="13" t="s">
+      <c r="L30" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M30" s="13">
+      <c r="M30" s="8">
         <v>0.15</v>
       </c>
-      <c r="N30" s="13">
+      <c r="N30" s="8">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:1024">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9" t="s">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="13">
+      <c r="J31" s="4"/>
+      <c r="K31" s="8">
         <v>3.14</v>
       </c>
-      <c r="L31" s="13">
+      <c r="L31" s="8">
         <v>2.62</v>
       </c>
-      <c r="M31" s="13">
+      <c r="M31" s="8">
         <v>1.99</v>
       </c>
-      <c r="N31" s="13" t="s">
+      <c r="N31" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:1024">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H32" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I32" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="13">
+      <c r="J32" s="4"/>
+      <c r="K32" s="8">
         <v>0.09</v>
       </c>
-      <c r="L32" s="13">
+      <c r="L32" s="8">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M32" s="13">
+      <c r="M32" s="8">
         <v>5.8500000000000003E-2</v>
       </c>
-      <c r="N32" s="13">
+      <c r="N32" s="8">
         <f>-C320603</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="4">
         <v>100</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J33" s="9"/>
-      <c r="K33" s="13">
+      <c r="J33" s="4"/>
+      <c r="K33" s="8">
         <v>0.08</v>
       </c>
-      <c r="L33" s="13">
+      <c r="L33" s="8">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="M33" s="13">
+      <c r="M33" s="8">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="N33" s="13">
+      <c r="N33" s="8">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="4">
         <v>649</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="12" t="s">
+      <c r="E34" s="4"/>
+      <c r="F34" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I34" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="J34" s="9"/>
-      <c r="K34" s="13">
+      <c r="J34" s="4"/>
+      <c r="K34" s="8">
         <v>0.1</v>
       </c>
-      <c r="L34" s="13">
+      <c r="L34" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M34" s="13">
+      <c r="M34" s="8">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="N34" s="13">
+      <c r="N34" s="8">
         <v>3.8400000000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="12" t="s">
+      <c r="E35" s="4"/>
+      <c r="F35" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="J35" s="9"/>
-      <c r="K35" s="13">
+      <c r="J35" s="4"/>
+      <c r="K35" s="8">
         <v>0.1</v>
       </c>
-      <c r="L35" s="13">
+      <c r="L35" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M35" s="13">
+      <c r="M35" s="8">
         <v>1.14E-2</v>
       </c>
-      <c r="N35" s="13">
+      <c r="N35" s="8">
         <v>4.1599999999999996E-3</v>
       </c>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="I36" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="13">
+      <c r="J36" s="4"/>
+      <c r="K36" s="8">
         <v>0.1</v>
       </c>
-      <c r="L36" s="13">
+      <c r="L36" s="8">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="M36" s="13">
+      <c r="M36" s="8">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="N36" s="13">
+      <c r="N36" s="8">
         <v>6.3E-3</v>
       </c>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="K37" s="15">
-        <v>1.77</v>
-      </c>
-      <c r="L37" s="15">
-        <v>1.46</v>
-      </c>
-      <c r="M37" s="15">
-        <v>1.0900000000000001</v>
+      <c r="K37" s="10">
+        <v>1.26</v>
+      </c>
+      <c r="L37" s="10">
+        <v>1.048</v>
+      </c>
+      <c r="M37" s="10">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="N37" s="10">
+        <v>0.50439999999999996</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G32" r:id="rId1"/>

</xml_diff>

<commit_message>
added 24pin 0.05" male header
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="29060" windowWidth="26420" windowHeight="14120" tabRatio="986"/>
+    <workbookView xWindow="3360" yWindow="2900" windowWidth="25600" windowHeight="16060" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="214">
   <si>
     <t>Part</t>
   </si>
@@ -652,6 +652,15 @@
   </si>
   <si>
     <t>S9015E-07-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER .050" 24PS DL PCB AU</t>
+  </si>
+  <si>
+    <t>GRPB122VWVN-RC</t>
+  </si>
+  <si>
+    <t>S9015E-12-ND</t>
   </si>
 </sst>
 </file>
@@ -784,19 +793,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1130,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK37"/>
+  <dimension ref="A1:AMK38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1153,19 +1162,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="14" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
@@ -1174,21 +1183,21 @@
       <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
       <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
@@ -2201,16 +2210,16 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="14"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="15"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -20694,19 +20703,48 @@
         <v>0.50439999999999996</v>
       </c>
     </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K38" s="10">
+        <v>1.93</v>
+      </c>
+      <c r="L38" s="10">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="M38" s="10">
+        <v>1.19</v>
+      </c>
+      <c r="N38" s="10">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G32" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated BOM and added data sheets for CAN and DAC ICs
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="227">
   <si>
     <t>Part</t>
   </si>
@@ -675,16 +675,38 @@
   </si>
   <si>
     <t>MAX3051ESA+-ND </t>
+  </si>
+  <si>
+    <t>4 output DAC</t>
+  </si>
+  <si>
+    <t>10-TFSOP </t>
+  </si>
+  <si>
+    <t>2.7-5.5V</t>
+  </si>
+  <si>
+    <t>IC DAC 12BIT QUAD R-R 10-MSOP </t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>DAC124S085CIMM/NOPB</t>
+  </si>
+  <si>
+    <t>DAC124S085CIMM/NOPBCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -725,12 +747,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -802,16 +830,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -823,7 +847,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -847,7 +871,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -859,12 +883,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -873,6 +917,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -892,10 +940,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -910,1324 +958,1324 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.5"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.5"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.1581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="2" width="7.16326530612245"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="7.16326530612245"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="8.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8" t="n">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="L2" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="M2" s="8" t="n">
+      <c r="M2" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="9" t="n">
+      <c r="N2" s="8" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="10" t="s">
+    <row r="3" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="14" t="n">
+      <c r="J3" s="9"/>
+      <c r="K3" s="13" t="n">
         <v>0.92</v>
       </c>
-      <c r="L3" s="14" t="n">
+      <c r="L3" s="13" t="n">
         <v>0.817</v>
       </c>
-      <c r="M3" s="14" t="n">
+      <c r="M3" s="13" t="n">
         <v>0.645</v>
       </c>
-      <c r="N3" s="14" t="n">
+      <c r="N3" s="13" t="n">
         <v>0.3968</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="14" t="n">
+      <c r="J4" s="9"/>
+      <c r="K4" s="13" t="n">
         <v>15.75</v>
       </c>
-      <c r="L4" s="14" t="n">
+      <c r="L4" s="13" t="n">
         <v>14.318</v>
       </c>
-      <c r="M4" s="14" t="n">
+      <c r="M4" s="13" t="n">
         <v>12.1703</v>
       </c>
-      <c r="N4" s="14" t="n">
+      <c r="N4" s="13" t="n">
         <v>9.52147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="14" t="n">
+      <c r="J5" s="9"/>
+      <c r="K5" s="13" t="n">
         <v>0.57</v>
       </c>
-      <c r="L5" s="14" t="n">
+      <c r="L5" s="13" t="n">
         <v>0.473</v>
       </c>
-      <c r="M5" s="14" t="n">
+      <c r="M5" s="13" t="n">
         <v>0.378</v>
       </c>
-      <c r="N5" s="14" t="n">
+      <c r="N5" s="13" t="n">
         <v>0.3024</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="14" t="n">
+      <c r="J6" s="9"/>
+      <c r="K6" s="13" t="n">
         <v>1.26</v>
       </c>
-      <c r="L6" s="14" t="n">
+      <c r="L6" s="13" t="n">
         <v>1.225</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="14" t="n">
+      <c r="J7" s="9"/>
+      <c r="K7" s="13" t="n">
         <v>1.49</v>
       </c>
-      <c r="L7" s="14" t="n">
+      <c r="L7" s="13" t="n">
         <v>1.24</v>
       </c>
-      <c r="M7" s="14" t="n">
+      <c r="M7" s="13" t="n">
         <v>0.94</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="14" t="n">
+      <c r="J8" s="9"/>
+      <c r="K8" s="13" t="n">
         <v>0.97</v>
       </c>
-      <c r="L8" s="14" t="n">
+      <c r="L8" s="13" t="n">
         <v>0.752</v>
       </c>
-      <c r="M8" s="14" t="n">
+      <c r="M8" s="13" t="n">
         <v>0.5738</v>
       </c>
-      <c r="N8" s="14" t="n">
+      <c r="N8" s="13" t="n">
         <v>0.408</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="15" t="n">
+      <c r="J9" s="9"/>
+      <c r="K9" s="14" t="n">
         <v>0.95</v>
       </c>
-      <c r="L9" s="15" t="n">
+      <c r="L9" s="14" t="n">
         <v>0.84</v>
       </c>
-      <c r="M9" s="15" t="n">
+      <c r="M9" s="14" t="n">
         <v>0.69</v>
       </c>
-      <c r="N9" s="15" t="n">
+      <c r="N9" s="14" t="n">
         <v>0.54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="14" t="n">
+      <c r="J10" s="9"/>
+      <c r="K10" s="13" t="n">
         <v>0.6</v>
       </c>
-      <c r="L10" s="14" t="n">
+      <c r="L10" s="13" t="n">
         <v>0.5</v>
       </c>
-      <c r="M10" s="14" t="n">
+      <c r="M10" s="13" t="n">
         <v>0.399</v>
       </c>
-      <c r="N10" s="14" t="n">
+      <c r="N10" s="13" t="n">
         <v>0.319</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="14" t="n">
+      <c r="J11" s="9"/>
+      <c r="K11" s="13" t="n">
         <v>0.4</v>
       </c>
-      <c r="L11" s="14" t="n">
+      <c r="L11" s="13" t="n">
         <v>0.31</v>
       </c>
-      <c r="M11" s="14" t="n">
+      <c r="M11" s="13" t="n">
         <v>0.216</v>
       </c>
-      <c r="N11" s="14" t="n">
+      <c r="N11" s="13" t="n">
         <v>0.11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="14" t="n">
+      <c r="J12" s="9"/>
+      <c r="K12" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L12" s="14" t="n">
+      <c r="L12" s="13" t="n">
         <v>0.025</v>
       </c>
-      <c r="M12" s="14" t="n">
+      <c r="M12" s="13" t="n">
         <v>0.0116</v>
       </c>
-      <c r="N12" s="14" t="n">
+      <c r="N12" s="13" t="n">
         <v>0.0063</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="14" t="n">
+      <c r="J13" s="9"/>
+      <c r="K13" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L13" s="14" t="n">
+      <c r="L13" s="13" t="n">
         <v>0.041</v>
       </c>
-      <c r="M13" s="14" t="n">
+      <c r="M13" s="13" t="n">
         <v>0.0187</v>
       </c>
-      <c r="N13" s="14" t="n">
+      <c r="N13" s="13" t="n">
         <v>0.0102</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="14" t="n">
+      <c r="J14" s="9"/>
+      <c r="K14" s="13" t="n">
         <v>0.17</v>
       </c>
-      <c r="L14" s="14" t="n">
+      <c r="L14" s="13" t="n">
         <v>0.115</v>
       </c>
-      <c r="M14" s="14" t="n">
+      <c r="M14" s="13" t="n">
         <v>0.546</v>
       </c>
-      <c r="N14" s="14" t="n">
+      <c r="N14" s="13" t="n">
         <v>0.3163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="14" t="n">
+      <c r="J15" s="9"/>
+      <c r="K15" s="13" t="n">
         <v>0.2</v>
       </c>
-      <c r="L15" s="14" t="n">
+      <c r="L15" s="13" t="n">
         <v>0.136</v>
       </c>
-      <c r="M15" s="14" t="n">
+      <c r="M15" s="13" t="n">
         <v>0.0693</v>
       </c>
-      <c r="N15" s="14" t="n">
+      <c r="N15" s="13" t="n">
         <v>0.04208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="14" t="n">
+      <c r="J16" s="9"/>
+      <c r="K16" s="13" t="n">
         <v>0.32</v>
       </c>
-      <c r="L16" s="14" t="n">
+      <c r="L16" s="13" t="n">
         <v>0.28</v>
       </c>
-      <c r="M16" s="14" t="n">
+      <c r="M16" s="13" t="n">
         <v>0.14</v>
       </c>
-      <c r="N16" s="14" t="n">
+      <c r="N16" s="13" t="n">
         <v>0.092</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="14" t="n">
+      <c r="J17" s="9"/>
+      <c r="K17" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M17" s="14" t="n">
+      <c r="M17" s="13" t="n">
         <v>0.0114</v>
       </c>
-      <c r="N17" s="14" t="n">
+      <c r="N17" s="13" t="n">
         <v>0.00416</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="14" t="n">
+      <c r="J18" s="9"/>
+      <c r="K18" s="13" t="n">
         <v>0.2</v>
       </c>
-      <c r="L18" s="14" t="n">
+      <c r="L18" s="13" t="n">
         <v>0.14</v>
       </c>
-      <c r="M18" s="14" t="n">
+      <c r="M18" s="13" t="n">
         <v>0.066</v>
       </c>
-      <c r="N18" s="14" t="n">
+      <c r="N18" s="13" t="n">
         <v>0.037</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="14" t="n">
+      <c r="J19" s="9"/>
+      <c r="K19" s="13" t="n">
         <v>0.48</v>
       </c>
-      <c r="L19" s="14" t="n">
+      <c r="L19" s="13" t="n">
         <v>0.45</v>
       </c>
-      <c r="M19" s="14" t="n">
+      <c r="M19" s="13" t="n">
         <v>0.35</v>
       </c>
-      <c r="N19" s="14" t="n">
+      <c r="N19" s="13" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="14" t="n">
+      <c r="J20" s="9"/>
+      <c r="K20" s="13" t="n">
         <v>0.21</v>
       </c>
-      <c r="L20" s="14" t="n">
+      <c r="L20" s="13" t="n">
         <v>0.2</v>
       </c>
-      <c r="M20" s="14" t="n">
+      <c r="M20" s="13" t="n">
         <v>0.18</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="13" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="14" t="n">
+      <c r="J21" s="9"/>
+      <c r="K21" s="13" t="n">
         <v>1.41</v>
       </c>
-      <c r="L21" s="14" t="n">
+      <c r="L21" s="13" t="n">
         <v>1.11</v>
       </c>
-      <c r="M21" s="14" t="n">
+      <c r="M21" s="13" t="n">
         <v>0.83</v>
       </c>
-      <c r="N21" s="14" t="n">
+      <c r="N21" s="13" t="n">
         <v>0.52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10" t="s">
+      <c r="I22" s="9"/>
+      <c r="J22" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="14" t="n">
+      <c r="K22" s="13" t="n">
         <v>1.79</v>
       </c>
-      <c r="L22" s="14" t="n">
+      <c r="L22" s="13" t="n">
         <v>1.16</v>
       </c>
-      <c r="M22" s="14" t="n">
+      <c r="M22" s="13" t="n">
         <v>1.03</v>
       </c>
-      <c r="N22" s="14" t="n">
+      <c r="N22" s="13" t="n">
         <v>0.677</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="13" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="14" t="n">
+      <c r="J23" s="9"/>
+      <c r="K23" s="13" t="n">
         <v>0.95</v>
       </c>
-      <c r="L23" s="14" t="n">
+      <c r="L23" s="13" t="n">
         <v>0.839</v>
       </c>
-      <c r="M23" s="14" t="n">
+      <c r="M23" s="13" t="n">
         <v>0.6934</v>
       </c>
-      <c r="N23" s="14" t="n">
+      <c r="N23" s="13" t="n">
         <v>0.54775</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="14" t="n">
+      <c r="J24" s="9"/>
+      <c r="K24" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L24" s="14" t="n">
+      <c r="L24" s="13" t="n">
         <v>0.061</v>
       </c>
-      <c r="M24" s="14" t="n">
+      <c r="M24" s="13" t="n">
         <v>0.0281</v>
       </c>
-      <c r="N24" s="14" t="n">
+      <c r="N24" s="13" t="n">
         <v>0.0153</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="10" t="n">
+      <c r="D25" s="9" t="n">
         <v>5.1</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J25" s="10"/>
-      <c r="K25" s="14" t="n">
+      <c r="J25" s="9"/>
+      <c r="K25" s="13" t="n">
         <v>0.07</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N25" s="14" t="n">
+      <c r="N25" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="10" t="n">
+      <c r="D26" s="9" t="n">
         <v>68</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="14" t="n">
+      <c r="J26" s="9"/>
+      <c r="K26" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L26" s="14" t="n">
+      <c r="L26" s="13" t="n">
         <v>0.01</v>
       </c>
-      <c r="M26" s="14" t="n">
+      <c r="M26" s="13" t="n">
         <v>0.01</v>
       </c>
-      <c r="N26" s="14" t="n">
+      <c r="N26" s="13" t="n">
         <v>0.01</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="14" t="n">
+      <c r="J27" s="9"/>
+      <c r="K27" s="13" t="n">
         <v>0.33</v>
       </c>
-      <c r="L27" s="14" t="n">
+      <c r="L27" s="13" t="n">
         <v>0.32</v>
       </c>
-      <c r="M27" s="14" t="n">
+      <c r="M27" s="13" t="n">
         <v>0.22</v>
       </c>
-      <c r="N27" s="14" t="n">
+      <c r="N27" s="13" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10" t="s">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="H28" s="10" t="n">
+      <c r="H28" s="9" t="n">
         <v>61300821021</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="14" t="n">
+      <c r="J28" s="9"/>
+      <c r="K28" s="13" t="n">
         <v>0.7</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="L28" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="14" t="n">
+      <c r="M28" s="13" t="n">
         <v>0.63</v>
       </c>
-      <c r="N28" s="14" t="s">
+      <c r="N28" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="14" t="n">
+      <c r="J29" s="9"/>
+      <c r="K29" s="13" t="n">
         <v>1.08</v>
       </c>
-      <c r="L29" s="14" t="n">
+      <c r="L29" s="13" t="n">
         <v>0.97</v>
       </c>
-      <c r="M29" s="14" t="n">
+      <c r="M29" s="13" t="n">
         <v>0.79</v>
       </c>
-      <c r="N29" s="14" t="n">
+      <c r="N29" s="13" t="n">
         <v>0.54</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="I30" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="14" t="n">
+      <c r="J30" s="9"/>
+      <c r="K30" s="13" t="n">
         <v>0.17</v>
       </c>
-      <c r="L30" s="14" t="s">
+      <c r="L30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M30" s="14" t="n">
+      <c r="M30" s="13" t="n">
         <v>0.15</v>
       </c>
-      <c r="N30" s="14" t="n">
+      <c r="N30" s="13" t="n">
         <v>0.14</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10" t="s">
+    <row r="31" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="I31" s="10" t="s">
+      <c r="I31" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="14" t="n">
+      <c r="J31" s="16"/>
+      <c r="K31" s="18" t="n">
         <v>3.14</v>
       </c>
-      <c r="L31" s="14" t="n">
+      <c r="L31" s="18" t="n">
         <v>2.62</v>
       </c>
-      <c r="M31" s="14" t="n">
+      <c r="M31" s="18" t="n">
         <v>1.99</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="N31" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="I32" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="14" t="n">
+      <c r="J32" s="9"/>
+      <c r="K32" s="13" t="n">
         <v>0.09</v>
       </c>
-      <c r="L32" s="14" t="n">
+      <c r="L32" s="13" t="n">
         <v>0.073</v>
       </c>
-      <c r="M32" s="14" t="n">
+      <c r="M32" s="13" t="n">
         <v>0.0585</v>
       </c>
-      <c r="N32" s="14" t="n">
+      <c r="N32" s="13" t="n">
         <f aca="false">-C320603</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="10" t="n">
+      <c r="D33" s="9" t="n">
         <v>100</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I33" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="14" t="n">
+      <c r="J33" s="9"/>
+      <c r="K33" s="13" t="n">
         <v>0.08</v>
       </c>
-      <c r="L33" s="14" t="n">
+      <c r="L33" s="13" t="n">
         <v>0.069</v>
       </c>
-      <c r="M33" s="14" t="n">
+      <c r="M33" s="13" t="n">
         <v>0.0408</v>
       </c>
-      <c r="N33" s="14" t="n">
+      <c r="N33" s="13" t="n">
         <v>0.024</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="10" t="n">
+      <c r="D34" s="9" t="n">
         <v>649</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="13" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="14" t="n">
+      <c r="J34" s="9"/>
+      <c r="K34" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L34" s="14" t="n">
+      <c r="L34" s="13" t="n">
         <v>0.025</v>
       </c>
-      <c r="M34" s="14" t="n">
+      <c r="M34" s="13" t="n">
         <v>0.0105</v>
       </c>
-      <c r="N34" s="14" t="n">
+      <c r="N34" s="13" t="n">
         <v>0.00384</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="13" t="s">
+      <c r="E35" s="9"/>
+      <c r="F35" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="I35" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="J35" s="10"/>
-      <c r="K35" s="14" t="n">
+      <c r="J35" s="9"/>
+      <c r="K35" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L35" s="14" t="n">
+      <c r="L35" s="13" t="n">
         <v>0.015</v>
       </c>
-      <c r="M35" s="14" t="n">
+      <c r="M35" s="13" t="n">
         <v>0.0114</v>
       </c>
-      <c r="N35" s="14" t="n">
+      <c r="N35" s="13" t="n">
         <v>0.00416</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F36" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="J36" s="10"/>
-      <c r="K36" s="14" t="n">
+      <c r="J36" s="9"/>
+      <c r="K36" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="L36" s="14" t="n">
+      <c r="L36" s="13" t="n">
         <v>0.026</v>
       </c>
-      <c r="M36" s="14" t="n">
+      <c r="M36" s="13" t="n">
         <v>0.011</v>
       </c>
-      <c r="N36" s="14" t="n">
+      <c r="N36" s="13" t="n">
         <v>0.0063</v>
       </c>
     </row>
@@ -2235,6 +2283,9 @@
       <c r="B37" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
       <c r="F37" s="1" t="s">
         <v>208</v>
       </c>
@@ -2247,16 +2298,16 @@
       <c r="I37" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="K37" s="2" t="n">
+      <c r="K37" s="19" t="n">
         <v>1.26</v>
       </c>
-      <c r="L37" s="2" t="n">
+      <c r="L37" s="19" t="n">
         <v>1.048</v>
       </c>
-      <c r="M37" s="2" t="n">
+      <c r="M37" s="19" t="n">
         <v>0.776</v>
       </c>
-      <c r="N37" s="2" t="n">
+      <c r="N37" s="19" t="n">
         <v>0.5044</v>
       </c>
     </row>
@@ -2264,6 +2315,9 @@
       <c r="B38" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
       <c r="F38" s="1" t="s">
         <v>211</v>
       </c>
@@ -2276,24 +2330,24 @@
       <c r="I38" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K38" s="2" t="n">
+      <c r="K38" s="19" t="n">
         <v>1.93</v>
       </c>
-      <c r="L38" s="2" t="n">
+      <c r="L38" s="19" t="n">
         <v>1.596</v>
       </c>
-      <c r="M38" s="2" t="n">
+      <c r="M38" s="19" t="n">
         <v>1.19</v>
       </c>
-      <c r="N38" s="2" t="n">
+      <c r="N38" s="19" t="n">
         <v>0.884</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="21" t="s">
         <v>215</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2302,29 +2356,64 @@
       <c r="E39" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="21" t="s">
         <v>217</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="I39" s="17" t="s">
+      <c r="I39" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="K39" s="2" t="n">
+      <c r="K39" s="19" t="n">
         <v>1.82</v>
       </c>
-      <c r="L39" s="2" t="n">
+      <c r="L39" s="19" t="n">
         <v>1.729</v>
       </c>
-      <c r="M39" s="2" t="n">
+      <c r="M39" s="19" t="n">
         <v>1.5556</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="N39" s="19" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="28.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="K40" s="22" t="n">
+        <v>6.97</v>
+      </c>
+      <c r="L40" s="22" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="M40" s="22" t="n">
+        <v>5.157</v>
+      </c>
+      <c r="N40" s="22" t="n">
+        <v>3.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 120 ohm resistor
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="0" windowWidth="18060" windowHeight="17560" tabRatio="986"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="245">
   <si>
     <t>Part</t>
   </si>
@@ -736,6 +736,24 @@
   </si>
   <si>
     <t>0.1uF</t>
+  </si>
+  <si>
+    <t>120 ohm resistor</t>
+  </si>
+  <si>
+    <t>120ohm</t>
+  </si>
+  <si>
+    <t>1/8 W</t>
+  </si>
+  <si>
+    <t>RES SMD 120 OHM 5% 1/8W 0402</t>
+  </si>
+  <si>
+    <t>CRCW0402120RJNEDHP</t>
+  </si>
+  <si>
+    <t>541-120YACT-ND</t>
   </si>
 </sst>
 </file>
@@ -899,19 +917,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1245,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK43"/>
+  <dimension ref="A1:AMK44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1268,19 +1286,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="20" t="s">
@@ -1289,33 +1307,33 @@
       <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="22"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="20"/>
-      <c r="C2" s="23"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -2829,19 +2847,57 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" s="1">
+        <v>402</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M44" s="1">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N44" s="1">
+        <v>2.3560000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>

<commit_message>
Added data sheets for tvs array and LMV344IDR. Updated mBOM to reflect changes
</commit_message>
<xml_diff>
--- a/mBom.xlsx
+++ b/mBom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="986"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="mBom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="254">
   <si>
     <t>Part</t>
   </si>
@@ -754,17 +754,45 @@
   </si>
   <si>
     <t>541-120YACT-ND</t>
+  </si>
+  <si>
+    <t>TVS array</t>
+  </si>
+  <si>
+    <t>14-UDFN</t>
+  </si>
+  <si>
+    <t>TVS Array</t>
+  </si>
+  <si>
+    <t>ESD8008MUTAG</t>
+  </si>
+  <si>
+    <t>ESD8008MUTAGOSCT-ND</t>
+  </si>
+  <si>
+    <t>LMV344IDR</t>
+  </si>
+  <si>
+    <t>14-SOIC</t>
+  </si>
+  <si>
+    <t>Rail-to-Rail Output CMOS Operational Amplifier</t>
+  </si>
+  <si>
+    <t>296-20925-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -779,8 +807,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -793,8 +828,14 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -857,11 +898,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -917,20 +973,30 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,6 +1004,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1263,42 +1334,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK44"/>
+  <dimension ref="A1:AMK46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="20" t="s">
@@ -1307,33 +1378,33 @@
       <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
       <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="22"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="2">
         <v>1</v>
       </c>
@@ -1347,7 +1418,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1384,7 +1455,7 @@
         <v>0.39679999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1421,7 +1492,7 @@
         <v>9.5214700000000008</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1">
+    <row r="5" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1456,7 +1527,7 @@
         <v>0.3024</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
@@ -1493,7 +1564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
@@ -1530,7 +1601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>44</v>
       </c>
@@ -1567,7 +1638,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>51</v>
       </c>
@@ -1604,7 +1675,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="9" customFormat="1">
+    <row r="10" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>56</v>
       </c>
@@ -1641,7 +1712,7 @@
         <v>0.31900000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>62</v>
       </c>
@@ -1678,7 +1749,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
@@ -1717,7 +1788,7 @@
         <v>6.3E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>77</v>
       </c>
@@ -1756,7 +1827,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>83</v>
       </c>
@@ -1795,7 +1866,7 @@
         <v>0.31630000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>89</v>
       </c>
@@ -1834,7 +1905,7 @@
         <v>4.2079999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>95</v>
       </c>
@@ -1873,7 +1944,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>101</v>
       </c>
@@ -1912,7 +1983,7 @@
         <v>4.1599999999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>108</v>
       </c>
@@ -1951,7 +2022,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>115</v>
       </c>
@@ -1984,7 +2055,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>120</v>
       </c>
@@ -2017,7 +2088,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>126</v>
       </c>
@@ -2054,7 +2125,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>133</v>
       </c>
@@ -2089,7 +2160,7 @@
         <v>0.67700000000000005</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="14" customHeight="1">
+    <row r="23" spans="2:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>139</v>
       </c>
@@ -2124,7 +2195,7 @@
         <v>0.54774999999999996</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>141</v>
       </c>
@@ -2163,7 +2234,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>147</v>
       </c>
@@ -2202,7 +2273,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>153</v>
       </c>
@@ -2241,7 +2312,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>157</v>
       </c>
@@ -2274,7 +2345,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>157</v>
       </c>
@@ -2307,7 +2378,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>157</v>
       </c>
@@ -2340,7 +2411,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>169</v>
       </c>
@@ -2375,7 +2446,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:14" s="9" customFormat="1">
+    <row r="31" spans="2:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>175</v>
       </c>
@@ -2410,7 +2481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>180</v>
       </c>
@@ -2450,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>186</v>
       </c>
@@ -2489,7 +2560,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>192</v>
       </c>
@@ -2526,7 +2597,7 @@
         <v>3.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>197</v>
       </c>
@@ -2563,7 +2634,7 @@
         <v>4.1599999999999996E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>202</v>
       </c>
@@ -2602,7 +2673,7 @@
         <v>6.3E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="15" customHeight="1">
+    <row r="37" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>157</v>
       </c>
@@ -2634,7 +2705,7 @@
         <v>0.50439999999999996</v>
       </c>
     </row>
-    <row r="38" spans="2:14" ht="15" customHeight="1">
+    <row r="38" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>157</v>
       </c>
@@ -2666,7 +2737,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="15" customHeight="1">
+    <row r="39" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="17" t="s">
         <v>214</v>
       </c>
@@ -2704,7 +2775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="15" customHeight="1">
+    <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>220</v>
       </c>
@@ -2739,7 +2810,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="41" spans="2:14" ht="15" customHeight="1">
+    <row r="41" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>227</v>
       </c>
@@ -2771,7 +2842,7 @@
         <v>0.42502000000000001</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="15" customHeight="1">
+    <row r="42" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>233</v>
       </c>
@@ -2796,20 +2867,20 @@
       <c r="I42" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="27">
         <v>0.1</v>
       </c>
-      <c r="L42" s="1">
+      <c r="L42" s="27">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M42" s="27">
         <v>2.1899999999999999E-2</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N42" s="27">
         <v>1.17E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:14" ht="15" customHeight="1">
+    <row r="43" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>237</v>
       </c>
@@ -2834,20 +2905,20 @@
       <c r="I43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="27">
         <v>0.1</v>
       </c>
-      <c r="L43" s="1">
+      <c r="L43" s="27">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M43" s="1">
+      <c r="M43" s="27">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="N43" s="1">
+      <c r="N43" s="27">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:14">
+    <row r="44" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>239</v>
       </c>
@@ -2872,34 +2943,99 @@
       <c r="I44" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="27">
         <v>0.17</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L44" s="27">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M44" s="27">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N44" s="27">
         <v>2.3560000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="K45" s="27">
+        <v>0.77</v>
+      </c>
+      <c r="L45" s="27">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="M45" s="27">
+        <v>0.51990000000000003</v>
+      </c>
+      <c r="N45" s="27">
+        <v>0.30854999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="K46" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="L46" s="27">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="M46" s="27">
+        <v>0.63</v>
+      </c>
+      <c r="N46" s="27">
+        <v>0.38750000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>